<commit_message>
2.1.3: Dynamic Clause: NOT IN and NOT BETWEEN are implemented.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoDbCommonResourceBundle.xlsx
+++ b/meta/program/BlancoDbCommonResourceBundle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoDbCommon/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8630737-E5E1-6647-8BC7-95EB5D950CAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F183E22-B7AC-4540-BD33-40D244410EB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="460" windowWidth="22000" windowHeight="16260" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
@@ -480,6 +480,29 @@
     </rPh>
     <rPh sb="43" eb="45">
       <t xml:space="preserve">セッテイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2JAVACLASS.ERR017</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SQL定義ID[{0}]のSQL動的条件式定義で条件句タイプ[{1}]は未定義です。</t>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">ドウテキ </t>
+    </rPh>
+    <rPh sb="18" eb="21">
+      <t xml:space="preserve">ジョウケンシキ </t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="24" eb="27">
+      <t xml:space="preserve">ジョウケンクタイプ </t>
+    </rPh>
+    <rPh sb="36" eb="39">
+      <t xml:space="preserve">ミテイギデス </t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1266,10 +1289,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1434,7 +1457,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="28">
-        <f t="shared" ref="A17:A54" si="0">A16+1</f>
+        <f t="shared" ref="A17:A55" si="0">A16+1</f>
         <v>3</v>
       </c>
       <c r="B17" s="23"/>
@@ -2001,13 +2024,29 @@
       <c r="G54" s="22"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="29"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="27"/>
+      <c r="A55" s="28">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="22"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="29"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="25"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2017,7 +2056,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D71" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D72" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
2.2.2: Implement FUNCTION for DynamicClause.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoDbCommonResourceBundle.xlsx
+++ b/meta/program/BlancoDbCommonResourceBundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoDbCommon/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F183E22-B7AC-4540-BD33-40D244410EB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B799A388-4F59-7F42-9DAE-30B5944EE9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="22000" windowHeight="16260" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="22000" windowHeight="16260" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ja" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
   <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
@@ -503,6 +503,210 @@
     </rPh>
     <rPh sb="36" eb="39">
       <t xml:space="preserve">ミテイギデス </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2JAVACLASS.ERR018</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2JAVACLASS.ERR019</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2JAVACLASS.ERR020</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SQL定義ID[{0}]のSQL動的条件式関数定義で関数タグ名が未定義です。</t>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">ドウテキ </t>
+    </rPh>
+    <rPh sb="18" eb="21">
+      <t xml:space="preserve">ジョウケンシキ </t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="32" eb="35">
+      <t xml:space="preserve">ミテイギデス </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SQL定義ID[{0}]のSQL動的条件式関数定義で関数タグ名[{1}]において関数名が設定されていません。</t>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">ドウテキ </t>
+    </rPh>
+    <rPh sb="18" eb="21">
+      <t xml:space="preserve">ジョウケンシキ </t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="32" eb="35">
+      <t xml:space="preserve">ミテイギデス </t>
+    </rPh>
+    <rPh sb="40" eb="43">
+      <t xml:space="preserve">カンスウメイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SQL定義ID[{0}]のSQL動的条件式関数定義で関数タグ名[{1}]においてパラメータ数が設定されていません。</t>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">ドウテキ </t>
+    </rPh>
+    <rPh sb="18" eb="21">
+      <t xml:space="preserve">ジョウケンシキ </t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="32" eb="35">
+      <t xml:space="preserve">ミテイギデス </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2JAVACLASS.ERR021</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SQL定義ID[{0}]のSQL動的条件式関数定義で関数タグ名[{1}]において不正なパラメータ数が指定されました。</t>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">ドウテキ </t>
+    </rPh>
+    <rPh sb="18" eb="21">
+      <t xml:space="preserve">ジョウケンシキ </t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="32" eb="35">
+      <t xml:space="preserve">ミテイギデス </t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t xml:space="preserve">フセイナ </t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2JAVACLASS.ERR022</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SQL定義ID[{0}]のSQL動的条件式関数定義で関数タグ名[{1}]においてパラメータ [{2}]の型が指定されていません。</t>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">ドウテキ </t>
+    </rPh>
+    <rPh sb="18" eb="21">
+      <t xml:space="preserve">ジョウケンシキ </t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="32" eb="35">
+      <t xml:space="preserve">ミテイギデス </t>
+    </rPh>
+    <rPh sb="52" eb="53">
+      <t xml:space="preserve">カタ </t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2JAVACLASS.ERR023</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SQL定義ID[{0}]のSQL動的条件式定義で条件句タイプFUNCTIONにおいて関数タグ[{1}]は未定義です。</t>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">ドウテキ </t>
+    </rPh>
+    <rPh sb="18" eb="21">
+      <t xml:space="preserve">ジョウケンシキ </t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="24" eb="27">
+      <t xml:space="preserve">ジョウケンクタイプ </t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="52" eb="55">
+      <t xml:space="preserve">ミテイギデス </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t># Excelメタファイル・チェック結果通知メッセージ</t>
+    <rPh sb="20" eb="22">
+      <t xml:space="preserve">ツウチ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2JAVACLASS.INFO001</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SQL定義ID[{0}]の動的関数定義[{1}]では試験実行のスキップが指定されています。</t>
+    <rPh sb="13" eb="15">
+      <t xml:space="preserve">ドウテキ </t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t xml:space="preserve">シケｎ </t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t xml:space="preserve">ジッコウ </t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t xml:space="preserve">シテイ </t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1289,10 +1493,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1457,7 +1661,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="28">
-        <f t="shared" ref="A17:A55" si="0">A16+1</f>
+        <f t="shared" ref="A17:A64" si="0">A16+1</f>
         <v>3</v>
       </c>
       <c r="B17" s="23"/>
@@ -2040,13 +2244,151 @@
       <c r="G55" s="22"/>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="29"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="27"/>
+      <c r="A56" s="28">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B56" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="22"/>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="28">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="22"/>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="28">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B58" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="22"/>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="28">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="22"/>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="28">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B60" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="22"/>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="28">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="22"/>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="28">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B62" s="23"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="22"/>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="28">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B63" s="23"/>
+      <c r="C63" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="22"/>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="28">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="22"/>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="29"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+      <c r="G65" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2056,7 +2398,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D72" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D81" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
2.2.3: Optimizer Hint MAX_EXECUTE_TIME is supported. * merge this commit into master branch after tranlation is done.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoDbCommonResourceBundle.xlsx
+++ b/meta/program/BlancoDbCommonResourceBundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoDbCommon/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B799A388-4F59-7F42-9DAE-30B5944EE9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2695ACA-A726-0B4E-A4D7-AC2786EFA481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="22000" windowHeight="16260" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="500" windowWidth="22000" windowHeight="16260" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ja" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
   <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
@@ -272,9 +272,6 @@
     <t>XML2JAVACLASS.ERR008</t>
   </si>
   <si>
-    <t>SQL定義ID[{0}]は「呼出型」でないのにSQL出力パラメータ{1}、パラメータID[{2}]が指定されています。</t>
-  </si>
-  <si>
     <t>XML2JAVACLASS.ERR009</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -707,6 +704,39 @@
     </rPh>
     <rPh sb="36" eb="38">
       <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XML2JAVACLASS.ERR024</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SQL定義ID[{0}]は「呼出型」でないのにSQL出力パラメータ{1}、パラメータID[{2}]が指定されています。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SQL定義ID[{0}]で「検索型」でないのにタイムアウト(MySQL)が「使用する」に設定されています。</t>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">ケンサク </t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">ドウテキ </t>
+    </rPh>
+    <rPh sb="18" eb="21">
+      <t xml:space="preserve">ジョウケンシキ </t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t xml:space="preserve">シヨウスル </t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t xml:space="preserve">セッテイ </t>
+    </rPh>
+    <rPh sb="46" eb="49">
+      <t xml:space="preserve">ミテイギデス </t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1493,10 +1523,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1661,7 +1691,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="28">
-        <f t="shared" ref="A17:A64" si="0">A16+1</f>
+        <f t="shared" ref="A17:A65" si="0">A16+1</f>
         <v>3</v>
       </c>
       <c r="B17" s="23"/>
@@ -1775,10 +1805,10 @@
         <v>11</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
@@ -1791,10 +1821,10 @@
         <v>12</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
@@ -1807,10 +1837,10 @@
         <v>13</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
@@ -1823,10 +1853,10 @@
         <v>14</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
@@ -2092,7 +2122,7 @@
         <v>49</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="D46" s="21"/>
       <c r="E46" s="21"/>
@@ -2105,10 +2135,10 @@
         <v>33</v>
       </c>
       <c r="B47" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="20" t="s">
         <v>51</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>52</v>
       </c>
       <c r="D47" s="35"/>
       <c r="E47" s="35"/>
@@ -2121,10 +2151,10 @@
         <v>34</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D48" s="21"/>
       <c r="E48" s="21"/>
@@ -2137,10 +2167,10 @@
         <v>35</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D49" s="21"/>
       <c r="E49" s="21"/>
@@ -2153,10 +2183,10 @@
         <v>36</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D50" s="21"/>
       <c r="E50" s="21"/>
@@ -2169,10 +2199,10 @@
         <v>37</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D51" s="21"/>
       <c r="E51" s="21"/>
@@ -2185,10 +2215,10 @@
         <v>38</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D52" s="21"/>
       <c r="E52" s="21"/>
@@ -2201,10 +2231,10 @@
         <v>39</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D53" s="21"/>
       <c r="E53" s="21"/>
@@ -2217,10 +2247,10 @@
         <v>40</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D54" s="21"/>
       <c r="E54" s="21"/>
@@ -2233,10 +2263,10 @@
         <v>41</v>
       </c>
       <c r="B55" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C55" s="20" t="s">
         <v>75</v>
-      </c>
-      <c r="C55" s="20" t="s">
-        <v>76</v>
       </c>
       <c r="D55" s="21"/>
       <c r="E55" s="21"/>
@@ -2249,10 +2279,10 @@
         <v>42</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D56" s="21"/>
       <c r="E56" s="21"/>
@@ -2265,10 +2295,10 @@
         <v>43</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D57" s="21"/>
       <c r="E57" s="21"/>
@@ -2281,10 +2311,10 @@
         <v>44</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D58" s="21"/>
       <c r="E58" s="21"/>
@@ -2297,10 +2327,10 @@
         <v>45</v>
       </c>
       <c r="B59" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C59" s="20" t="s">
         <v>83</v>
-      </c>
-      <c r="C59" s="20" t="s">
-        <v>84</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="21"/>
@@ -2313,10 +2343,10 @@
         <v>46</v>
       </c>
       <c r="B60" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C60" s="20" t="s">
         <v>85</v>
-      </c>
-      <c r="C60" s="20" t="s">
-        <v>86</v>
       </c>
       <c r="D60" s="21"/>
       <c r="E60" s="21"/>
@@ -2329,10 +2359,10 @@
         <v>47</v>
       </c>
       <c r="B61" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="20" t="s">
         <v>87</v>
-      </c>
-      <c r="C61" s="20" t="s">
-        <v>88</v>
       </c>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
@@ -2344,8 +2374,12 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B62" s="23"/>
-      <c r="C62" s="20"/>
+      <c r="B62" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>93</v>
+      </c>
       <c r="D62" s="21"/>
       <c r="E62" s="21"/>
       <c r="F62" s="21"/>
@@ -2357,9 +2391,7 @@
         <v>49</v>
       </c>
       <c r="B63" s="23"/>
-      <c r="C63" s="20" t="s">
-        <v>89</v>
-      </c>
+      <c r="C63" s="20"/>
       <c r="D63" s="21"/>
       <c r="E63" s="21"/>
       <c r="F63" s="21"/>
@@ -2370,11 +2402,9 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B64" s="23" t="s">
-        <v>90</v>
-      </c>
+      <c r="B64" s="23"/>
       <c r="C64" s="20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D64" s="21"/>
       <c r="E64" s="21"/>
@@ -2382,13 +2412,29 @@
       <c r="G64" s="22"/>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="29"/>
-      <c r="B65" s="24"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="26"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="26"/>
-      <c r="G65" s="27"/>
+      <c r="A65" s="28">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="22"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="29"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="26"/>
+      <c r="G66" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2398,7 +2444,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D81" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D82" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>